<commit_message>
Override de save en LugarForm
</commit_message>
<xml_diff>
--- a/static/files/TemplateCargaMasiva.xlsx
+++ b/static/files/TemplateCargaMasiva.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Codigo postal</t>
   </si>
   <si>
-    <t xml:space="preserve">ID curso</t>
+    <t xml:space="preserve">ID grupo</t>
   </si>
 </sst>
 </file>
@@ -175,8 +175,8 @@
   </sheetPr>
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>